<commit_message>
Big Updates to I125 Binding
No longer need to manually add the Decay Factor into the ligand database, the python script will determine the difference between todays date and the calibration date, and use that number in a formula to determine the Decay Factor.

Additionally, the radioactivity archive sheet will have the calibration date and decay factor added to it

And, if it is someone's first time using the 125I python script, it will automatically move the blank copies of the radioactive waste disposal and archive sheet into the root folder of the 125I binding

Fingers crossed I haven't irreperably done anything
</commit_message>
<xml_diff>
--- a/Python_Scripts/I125_Binding/data_files/125I-Radioactivity_Archive_blank.xlsx
+++ b/Python_Scripts/I125_Binding/data_files/125I-Radioactivity_Archive_blank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kealbert\Documents\Python Scripts\Trying stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kealbert\Documents\Python Scripts\Trying stuff\I125_Binding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7729E8B7-6CAF-4027-AE86-CCEA2EFA49BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9523F-2131-4870-AED3-6AB2574FC912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Binding Type</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>SEC Pellet/Plate</t>
+  </si>
+  <si>
+    <t>Calibration Date</t>
+  </si>
+  <si>
+    <t>Decay Factor</t>
   </si>
 </sst>
 </file>
@@ -519,11 +525,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH1"/>
+  <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A476" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,9 +555,10 @@
     <col min="31" max="31" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="7.140625" customWidth="1"/>
     <col min="34" max="34" width="7.28515625" customWidth="1"/>
+    <col min="35" max="35" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -641,6 +648,12 @@
       </c>
       <c r="AH1" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>